<commit_message>
pushLogin and change excel type
</commit_message>
<xml_diff>
--- a/src/ciobrain-api/src/data/Infrastructure.xlsx
+++ b/src/ciobrain-api/src/data/Infrastructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00000S22-CIObrain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SpeedyNS.SPEEDYNS\Google Drive\Documents\Programming\CIOBrain\ciobrain-mono\src\ciobrain-api\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3B1966E-C5FF-42A5-9606-FF19C384C7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AF0788-BD93-49C7-B4A1-467C95F49040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="918" windowWidth="20208" windowHeight="12042" xr2:uid="{DC75A604-7F14-4874-ACAD-732E5A706C0E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{DC75A604-7F14-4874-ACAD-732E5A706C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <t>server-3</t>
   </si>
   <si>
-    <t>Long Type</t>
-  </si>
-  <si>
     <t>Short Type</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>Swit</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -298,12 +298,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,36 +648,35 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.47265625" style="4" customWidth="1"/>
-    <col min="2" max="3" width="12.26171875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.26171875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.47265625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.26171875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.3671875" style="4" customWidth="1"/>
-    <col min="8" max="9" width="15.15625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="10.1015625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="14.68359375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="14.62890625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12" style="4" customWidth="1"/>
-    <col min="14" max="14" width="16.83984375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="13.15625" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="8.83984375" style="4"/>
+    <col min="1" max="1" width="14.46484375" customWidth="1"/>
+    <col min="2" max="3" width="12.265625" customWidth="1"/>
+    <col min="4" max="4" width="15.265625" customWidth="1"/>
+    <col min="5" max="5" width="22.46484375" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="9" width="15.1328125" customWidth="1"/>
+    <col min="10" max="10" width="10.06640625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="16.86328125" customWidth="1"/>
+    <col min="15" max="15" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -717,7 +715,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -725,7 +723,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
@@ -759,7 +757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -767,7 +765,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>46</v>
@@ -801,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -809,7 +807,7 @@
         <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>47</v>
@@ -841,7 +839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -849,7 +847,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>41</v>
@@ -865,7 +863,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -873,7 +871,7 @@
         <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>44</v>
@@ -891,7 +889,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -899,7 +897,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -913,7 +911,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -921,7 +919,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -935,7 +933,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -943,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
@@ -967,7 +965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>

</xml_diff>